<commit_message>
reorganized things. Fixed a thing
</commit_message>
<xml_diff>
--- a/Wheat-price-data.xlsx
+++ b/Wheat-price-data.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="212">
   <si>
     <t>Month</t>
   </si>
@@ -23,9 +23,6 @@
   </si>
   <si>
     <t>106.88</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>111.77</t>
@@ -658,7 +655,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -734,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -749,6 +749,12 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -769,7 +775,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -783,7 +789,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -809,7 +814,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2136,6 +2141,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0C31-4B01-A28F-7FCE25FC1627}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2145,11 +2155,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="279702856"/>
-        <c:axId val="280101984"/>
+        <c:axId val="373073984"/>
+        <c:axId val="292024856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="279702856"/>
+        <c:axId val="373073984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2203,15 +2213,15 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280101984"/>
+        <c:crossAx val="292024856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="280101984"/>
+        <c:axId val="292024856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2265,10 +2275,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="279702856"/>
+        <c:crossAx val="373073984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2306,7 +2316,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2984,6 +2994,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3019,6 +3046,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3197,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="F215" sqref="F215"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3215,7 +3259,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3225,8 +3269,8 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
+      <c r="C2" s="6">
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3234,9 +3278,9 @@
         <v>36100</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7">
         <f>(B3-B2)/B2</f>
         <v>4.5752245508982041E-2</v>
       </c>
@@ -3246,9 +3290,9 @@
         <v>36130</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7">
         <f>(B4-B3)/B3</f>
         <v>-3.6056186812203642E-2</v>
       </c>
@@ -3258,9 +3302,9 @@
         <v>36161</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
         <f>(B5-B4)/B4</f>
         <v>1.8563207722294677E-3</v>
       </c>
@@ -3270,9 +3314,9 @@
         <v>36192</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7">
         <f t="shared" ref="C6:C69" si="0">(B6-B5)/B5</f>
         <v>-3.2518065591995472E-2</v>
       </c>
@@ -3282,9 +3326,9 @@
         <v>36220</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7">
         <f t="shared" si="0"/>
         <v>3.2557694149190762E-2</v>
       </c>
@@ -3294,9 +3338,9 @@
         <v>36251</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7">
         <f t="shared" si="0"/>
         <v>-1.3447092645831427E-2</v>
       </c>
@@ -3306,9 +3350,9 @@
         <v>36281</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7">
         <f t="shared" si="0"/>
         <v>-3.7601052829471746E-4</v>
       </c>
@@ -3318,9 +3362,9 @@
         <v>36312</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7">
         <f t="shared" si="0"/>
         <v>9.5918751175474506E-3</v>
       </c>
@@ -3330,9 +3374,9 @@
         <v>36342</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="5">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7">
         <f t="shared" si="0"/>
         <v>-7.2745901639344288E-2</v>
       </c>
@@ -3342,9 +3386,9 @@
         <v>36373</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5">
+        <v>12</v>
+      </c>
+      <c r="C12" s="7">
         <f t="shared" si="0"/>
         <v>5.5549974886991475E-2</v>
       </c>
@@ -3354,9 +3398,9 @@
         <v>36404</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7">
         <f t="shared" si="0"/>
         <v>2.5885039969547E-2</v>
       </c>
@@ -3366,9 +3410,9 @@
         <v>36434</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="5">
+        <v>14</v>
+      </c>
+      <c r="C14" s="7">
         <f t="shared" si="0"/>
         <v>-6.3265306122448919E-2</v>
       </c>
@@ -3378,9 +3422,9 @@
         <v>36465</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="5">
+        <v>15</v>
+      </c>
+      <c r="C15" s="7">
         <f t="shared" si="0"/>
         <v>4.238463061992475E-2</v>
       </c>
@@ -3390,9 +3434,9 @@
         <v>36495</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="5">
+        <v>16</v>
+      </c>
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>-3.9996199885996654E-2</v>
       </c>
@@ -3402,9 +3446,9 @@
         <v>36526</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="5">
+        <v>6</v>
+      </c>
+      <c r="C17" s="7">
         <f t="shared" si="0"/>
         <v>3.3448787728847199E-2</v>
       </c>
@@ -3414,9 +3458,9 @@
         <v>36557</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="5">
+        <v>17</v>
+      </c>
+      <c r="C18" s="7">
         <f t="shared" si="0"/>
         <v>5.57311117494972E-2</v>
       </c>
@@ -3426,9 +3470,9 @@
         <v>36586</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="5">
+        <v>18</v>
+      </c>
+      <c r="C19" s="7">
         <f t="shared" si="0"/>
         <v>-5.8049886621315246E-3</v>
       </c>
@@ -3438,9 +3482,9 @@
         <v>36617</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="5">
+        <v>19</v>
+      </c>
+      <c r="C20" s="7">
         <f t="shared" si="0"/>
         <v>1.2955022351975201E-2</v>
       </c>
@@ -3450,9 +3494,9 @@
         <v>36647</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="5">
+        <v>20</v>
+      </c>
+      <c r="C21" s="7">
         <f t="shared" si="0"/>
         <v>0.10150409799153379</v>
       </c>
@@ -3462,9 +3506,9 @@
         <v>36678</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="5">
+        <v>21</v>
+      </c>
+      <c r="C22" s="7">
         <f t="shared" si="0"/>
         <v>-2.2076860179885551E-2</v>
       </c>
@@ -3474,9 +3518,9 @@
         <v>36708</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="5">
+        <v>22</v>
+      </c>
+      <c r="C23" s="7">
         <f t="shared" si="0"/>
         <v>-3.0183946488294311E-2</v>
       </c>
@@ -3486,9 +3530,9 @@
         <v>36739</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="5">
+        <v>23</v>
+      </c>
+      <c r="C24" s="7">
         <f t="shared" si="0"/>
         <v>3.2675230623329651E-2</v>
       </c>
@@ -3498,9 +3542,9 @@
         <v>36770</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="5">
+        <v>24</v>
+      </c>
+      <c r="C25" s="7">
         <f t="shared" si="0"/>
         <v>0.12497912840207046</v>
       </c>
@@ -3510,9 +3554,9 @@
         <v>36800</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="5">
+        <v>25</v>
+      </c>
+      <c r="C26" s="7">
         <f t="shared" si="0"/>
         <v>0.11317254174397032</v>
       </c>
@@ -3522,9 +3566,9 @@
         <v>36831</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="5">
+        <v>26</v>
+      </c>
+      <c r="C27" s="7">
         <f t="shared" si="0"/>
         <v>-5.5333333333334169E-3</v>
       </c>
@@ -3534,9 +3578,9 @@
         <v>36861</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="5">
+        <v>27</v>
+      </c>
+      <c r="C28" s="7">
         <f t="shared" si="0"/>
         <v>-3.9284038345511738E-2</v>
       </c>
@@ -3546,9 +3590,9 @@
         <v>36892</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="5">
+        <v>28</v>
+      </c>
+      <c r="C29" s="7">
         <f t="shared" si="0"/>
         <v>-1.1932175005233466E-2</v>
       </c>
@@ -3558,9 +3602,9 @@
         <v>36923</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="5">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7">
         <f t="shared" si="0"/>
         <v>-1.8149717514124246E-2</v>
       </c>
@@ -3570,9 +3614,9 @@
         <v>36951</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="5">
+        <v>30</v>
+      </c>
+      <c r="C31" s="7">
         <f t="shared" si="0"/>
         <v>3.0712795799467812E-2</v>
       </c>
@@ -3582,9 +3626,9 @@
         <v>36982</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="5">
+        <v>31</v>
+      </c>
+      <c r="C32" s="7">
         <f t="shared" si="0"/>
         <v>1.1653872993719382E-2</v>
       </c>
@@ -3594,9 +3638,9 @@
         <v>37012</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="5">
+        <v>32</v>
+      </c>
+      <c r="C33" s="7">
         <f t="shared" si="0"/>
         <v>6.5530799475753604E-2</v>
       </c>
@@ -3606,9 +3650,9 @@
         <v>37043</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="5">
+        <v>33</v>
+      </c>
+      <c r="C34" s="7">
         <f t="shared" si="0"/>
         <v>-3.4569819382404374E-2</v>
       </c>
@@ -3618,9 +3662,9 @@
         <v>37073</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="5">
+        <v>34</v>
+      </c>
+      <c r="C35" s="7">
         <f t="shared" si="0"/>
         <v>-3.5338295446925377E-2</v>
       </c>
@@ -3630,9 +3674,9 @@
         <v>37104</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="5">
+        <v>35</v>
+      </c>
+      <c r="C36" s="7">
         <f t="shared" si="0"/>
         <v>-5.8598637564298665E-2</v>
       </c>
@@ -3642,9 +3686,9 @@
         <v>37135</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="5">
+        <v>36</v>
+      </c>
+      <c r="C37" s="7">
         <f t="shared" si="0"/>
         <v>-1.0854315882743845E-2</v>
       </c>
@@ -3654,9 +3698,9 @@
         <v>37165</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="5">
+        <v>37</v>
+      </c>
+      <c r="C38" s="7">
         <f t="shared" si="0"/>
         <v>1.6497461928933855E-2</v>
       </c>
@@ -3666,9 +3710,9 @@
         <v>37196</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="5">
+        <v>38</v>
+      </c>
+      <c r="C39" s="7">
         <f t="shared" si="0"/>
         <v>3.5837555996181422E-2</v>
       </c>
@@ -3678,9 +3722,9 @@
         <v>37226</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="5">
+        <v>39</v>
+      </c>
+      <c r="C40" s="7">
         <f t="shared" si="0"/>
         <v>-2.6444523218716893E-2</v>
       </c>
@@ -3690,9 +3734,9 @@
         <v>37257</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="5">
+        <v>40</v>
+      </c>
+      <c r="C41" s="7">
         <f t="shared" si="0"/>
         <v>3.3352752694436445E-2</v>
       </c>
@@ -3702,9 +3746,9 @@
         <v>37288</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C42" s="5">
+        <v>41</v>
+      </c>
+      <c r="C42" s="7">
         <f t="shared" si="0"/>
         <v>-1.4094432699085064E-3</v>
       </c>
@@ -3714,9 +3758,9 @@
         <v>37316</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C43" s="5">
+        <v>42</v>
+      </c>
+      <c r="C43" s="7">
         <f t="shared" si="0"/>
         <v>-1.2350035285815103E-2</v>
       </c>
@@ -3726,9 +3770,9 @@
         <v>37347</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="5">
+        <v>43</v>
+      </c>
+      <c r="C44" s="7">
         <f t="shared" si="0"/>
         <v>-2.0007145409074753E-3</v>
       </c>
@@ -3738,9 +3782,9 @@
         <v>37377</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C45" s="5">
+        <v>44</v>
+      </c>
+      <c r="C45" s="7">
         <f t="shared" si="0"/>
         <v>-5.1621679673516004E-2</v>
       </c>
@@ -3750,9 +3794,9 @@
         <v>37408</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" s="5">
+        <v>45</v>
+      </c>
+      <c r="C46" s="7">
         <f t="shared" si="0"/>
         <v>4.3635814585535261E-2</v>
       </c>
@@ -3762,9 +3806,9 @@
         <v>37438</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" s="5">
+        <v>46</v>
+      </c>
+      <c r="C47" s="7">
         <f t="shared" si="0"/>
         <v>8.8686342592592518E-2</v>
       </c>
@@ -3774,9 +3818,9 @@
         <v>37469</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="5">
+        <v>47</v>
+      </c>
+      <c r="C48" s="7">
         <f t="shared" si="0"/>
         <v>9.6212624584717535E-2</v>
       </c>
@@ -3786,9 +3830,9 @@
         <v>37500</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C49" s="5">
+        <v>48</v>
+      </c>
+      <c r="C49" s="7">
         <f t="shared" si="0"/>
         <v>0.16092859740574622</v>
       </c>
@@ -3798,9 +3842,9 @@
         <v>37530</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50" s="5">
+        <v>49</v>
+      </c>
+      <c r="C50" s="7">
         <f t="shared" si="0"/>
         <v>1.3104996606275732E-2</v>
       </c>
@@ -3810,9 +3854,9 @@
         <v>37561</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C51" s="5">
+        <v>50</v>
+      </c>
+      <c r="C51" s="7">
         <f t="shared" si="0"/>
         <v>-9.3176664605235951E-2</v>
       </c>
@@ -3822,9 +3866,9 @@
         <v>37591</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C52" s="5">
+        <v>51</v>
+      </c>
+      <c r="C52" s="7">
         <f t="shared" si="0"/>
         <v>-5.6660604682882462E-2</v>
       </c>
@@ -3834,9 +3878,9 @@
         <v>37622</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" s="5">
+        <v>52</v>
+      </c>
+      <c r="C53" s="7">
         <f t="shared" si="0"/>
         <v>-0.15133441773600823</v>
       </c>
@@ -3846,9 +3890,9 @@
         <v>37653</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="5">
+        <v>53</v>
+      </c>
+      <c r="C54" s="7">
         <f t="shared" si="0"/>
         <v>-6.0339319940370152E-3</v>
       </c>
@@ -3858,9 +3902,9 @@
         <v>37681</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C55" s="5">
+        <v>54</v>
+      </c>
+      <c r="C55" s="7">
         <f t="shared" si="0"/>
         <v>-6.2562491072704035E-2</v>
       </c>
@@ -3870,9 +3914,9 @@
         <v>37712</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="5">
+        <v>55</v>
+      </c>
+      <c r="C56" s="7">
         <f t="shared" si="0"/>
         <v>-2.6283711717202413E-2</v>
       </c>
@@ -3882,9 +3926,9 @@
         <v>37742</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="5">
+        <v>56</v>
+      </c>
+      <c r="C57" s="7">
         <f t="shared" si="0"/>
         <v>-4.0763633518504094E-2</v>
       </c>
@@ -3894,9 +3938,9 @@
         <v>37773</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="5">
+        <v>57</v>
+      </c>
+      <c r="C58" s="7">
         <f t="shared" si="0"/>
         <v>-8.1239804241435509E-2</v>
       </c>
@@ -3906,9 +3950,9 @@
         <v>37803</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C59" s="5">
+        <v>58</v>
+      </c>
+      <c r="C59" s="7">
         <f t="shared" si="0"/>
         <v>2.7610085227272721E-2</v>
       </c>
@@ -3918,9 +3962,9 @@
         <v>37834</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C60" s="5">
+        <v>59</v>
+      </c>
+      <c r="C60" s="7">
         <f t="shared" si="0"/>
         <v>0.15386609071274299</v>
       </c>
@@ -3930,9 +3974,9 @@
         <v>37865</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C61" s="5">
+        <v>60</v>
+      </c>
+      <c r="C61" s="7">
         <f t="shared" si="0"/>
         <v>-2.8002395926924297E-2</v>
       </c>
@@ -3942,9 +3986,9 @@
         <v>37895</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C62" s="5">
+        <v>61</v>
+      </c>
+      <c r="C62" s="7">
         <f t="shared" si="0"/>
         <v>-2.8423971653058065E-2</v>
       </c>
@@ -3954,9 +3998,9 @@
         <v>37926</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="5">
+        <v>62</v>
+      </c>
+      <c r="C63" s="7">
         <f t="shared" si="0"/>
         <v>8.8004439863632725E-2</v>
       </c>
@@ -3966,9 +4010,9 @@
         <v>37956</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" s="5">
+        <v>63</v>
+      </c>
+      <c r="C64" s="7">
         <f t="shared" si="0"/>
         <v>-1.7780368724039916E-2</v>
       </c>
@@ -3978,9 +4022,9 @@
         <v>37987</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C65" s="5">
+        <v>64</v>
+      </c>
+      <c r="C65" s="7">
         <f t="shared" si="0"/>
         <v>-2.1589138660137969E-2</v>
       </c>
@@ -3990,9 +4034,9 @@
         <v>38018</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" s="5">
+        <v>65</v>
+      </c>
+      <c r="C66" s="7">
         <f t="shared" si="0"/>
         <v>-3.2226266302699424E-2</v>
       </c>
@@ -4002,9 +4046,9 @@
         <v>38047</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C67" s="5">
+        <v>66</v>
+      </c>
+      <c r="C67" s="7">
         <f t="shared" si="0"/>
         <v>6.2602836323748412E-2</v>
       </c>
@@ -4014,9 +4058,9 @@
         <v>38078</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C68" s="5">
+        <v>67</v>
+      </c>
+      <c r="C68" s="7">
         <f t="shared" si="0"/>
         <v>2.4922577790886264E-2</v>
       </c>
@@ -4026,9 +4070,9 @@
         <v>38108</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C69" s="5">
+        <v>68</v>
+      </c>
+      <c r="C69" s="7">
         <f t="shared" si="0"/>
         <v>-1.8129496402877771E-2</v>
       </c>
@@ -4038,9 +4082,9 @@
         <v>38139</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C70" s="5">
+        <v>69</v>
+      </c>
+      <c r="C70" s="7">
         <f t="shared" ref="C70:C133" si="1">(B70-B69)/B69</f>
         <v>-6.6236811254396191E-2</v>
       </c>
@@ -4050,9 +4094,9 @@
         <v>38169</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C71" s="5">
+        <v>70</v>
+      </c>
+      <c r="C71" s="7">
         <f t="shared" si="1"/>
         <v>-3.6487758945386001E-2</v>
       </c>
@@ -4062,9 +4106,9 @@
         <v>38200</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C72" s="5">
+        <v>71</v>
+      </c>
+      <c r="C72" s="7">
         <f t="shared" si="1"/>
         <v>-5.48904633927845E-2</v>
       </c>
@@ -4074,9 +4118,9 @@
         <v>38231</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C73" s="5">
+        <v>72</v>
+      </c>
+      <c r="C73" s="7">
         <f t="shared" si="1"/>
         <v>6.5230504093063399E-2</v>
       </c>
@@ -4086,9 +4130,9 @@
         <v>38261</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C74" s="5">
+        <v>73</v>
+      </c>
+      <c r="C74" s="7">
         <f t="shared" si="1"/>
         <v>-2.7260961009545417E-2</v>
       </c>
@@ -4098,9 +4142,9 @@
         <v>38292</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C75" s="5">
+        <v>74</v>
+      </c>
+      <c r="C75" s="7">
         <f t="shared" si="1"/>
         <v>2.4116424116424635E-3</v>
       </c>
@@ -4110,9 +4154,9 @@
         <v>38322</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C76" s="5">
+        <v>75</v>
+      </c>
+      <c r="C76" s="7">
         <f t="shared" si="1"/>
         <v>-4.7867927658868506E-2</v>
       </c>
@@ -4122,9 +4166,9 @@
         <v>38353</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C77" s="5">
+        <v>76</v>
+      </c>
+      <c r="C77" s="7">
         <f t="shared" si="1"/>
         <v>2.0127210943626402E-2</v>
       </c>
@@ -4134,9 +4178,9 @@
         <v>38384</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C78" s="5">
+        <v>77</v>
+      </c>
+      <c r="C78" s="7">
         <f t="shared" si="1"/>
         <v>-6.9183464297916152E-3</v>
       </c>
@@ -4146,9 +4190,9 @@
         <v>38412</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C79" s="5">
+        <v>78</v>
+      </c>
+      <c r="C79" s="7">
         <f t="shared" si="1"/>
         <v>-1.6083254493850438E-2</v>
       </c>
@@ -4158,9 +4202,9 @@
         <v>38443</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C80" s="5">
+        <v>79</v>
+      </c>
+      <c r="C80" s="7">
         <f t="shared" si="1"/>
         <v>-4.8164335664335707E-2</v>
       </c>
@@ -4170,9 +4214,9 @@
         <v>38473</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C81" s="5">
+        <v>80</v>
+      </c>
+      <c r="C81" s="7">
         <f t="shared" si="1"/>
         <v>4.3805675452291269E-2</v>
       </c>
@@ -4182,9 +4226,9 @@
         <v>38504</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C82" s="5">
+        <v>81</v>
+      </c>
+      <c r="C82" s="7">
         <f t="shared" si="1"/>
         <v>2.657047334154505E-2</v>
       </c>
@@ -4194,9 +4238,9 @@
         <v>38534</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C83" s="5">
+        <v>82</v>
+      </c>
+      <c r="C83" s="7">
         <f t="shared" si="1"/>
         <v>2.4425779910867279E-2</v>
       </c>
@@ -4206,9 +4250,9 @@
         <v>38565</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C84" s="5">
+        <v>83</v>
+      </c>
+      <c r="C84" s="7">
         <f t="shared" si="1"/>
         <v>1.6564879109846935E-2</v>
       </c>
@@ -4218,9 +4262,9 @@
         <v>38596</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C85" s="5">
+        <v>84</v>
+      </c>
+      <c r="C85" s="7">
         <f t="shared" si="1"/>
         <v>7.2586618385318144E-2</v>
       </c>
@@ -4230,9 +4274,9 @@
         <v>38626</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C86" s="5">
+        <v>85</v>
+      </c>
+      <c r="C86" s="7">
         <f t="shared" si="1"/>
         <v>7.1817693547149425E-2</v>
       </c>
@@ -4242,9 +4286,9 @@
         <v>38657</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C87" s="5">
+        <v>86</v>
+      </c>
+      <c r="C87" s="7">
         <f t="shared" si="1"/>
         <v>-2.1261364449853239E-2</v>
       </c>
@@ -4254,9 +4298,9 @@
         <v>38687</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C88" s="5">
+        <v>87</v>
+      </c>
+      <c r="C88" s="7">
         <f t="shared" si="1"/>
         <v>1.4482153306026842E-2</v>
       </c>
@@ -4266,9 +4310,9 @@
         <v>38718</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C89" s="5">
+        <v>88</v>
+      </c>
+      <c r="C89" s="7">
         <f t="shared" si="1"/>
         <v>-4.1816870944483353E-3</v>
       </c>
@@ -4278,9 +4322,9 @@
         <v>38749</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C90" s="5">
+        <v>89</v>
+      </c>
+      <c r="C90" s="7">
         <f t="shared" si="1"/>
         <v>9.0718216044019695E-2</v>
       </c>
@@ -4290,9 +4334,9 @@
         <v>38777</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C91" s="5">
+        <v>90</v>
+      </c>
+      <c r="C91" s="7">
         <f t="shared" si="1"/>
         <v>-3.6641221374045865E-2</v>
       </c>
@@ -4302,9 +4346,9 @@
         <v>38808</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C92" s="5">
+        <v>91</v>
+      </c>
+      <c r="C92" s="7">
         <f t="shared" si="1"/>
         <v>1.2816095914008225E-2</v>
       </c>
@@ -4314,9 +4358,9 @@
         <v>38838</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C93" s="5">
+        <v>92</v>
+      </c>
+      <c r="C93" s="7">
         <f t="shared" si="1"/>
         <v>2.9185658888359698E-2</v>
       </c>
@@ -4326,9 +4370,9 @@
         <v>38869</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C94" s="5">
+        <v>93</v>
+      </c>
+      <c r="C94" s="7">
         <f t="shared" si="1"/>
         <v>1.9896879957694281E-2</v>
       </c>
@@ -4338,9 +4382,9 @@
         <v>38899</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C95" s="5">
+        <v>94</v>
+      </c>
+      <c r="C95" s="7">
         <f t="shared" si="1"/>
         <v>3.4480523689156925E-2</v>
       </c>
@@ -4350,9 +4394,9 @@
         <v>38930</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C96" s="5">
+        <v>95</v>
+      </c>
+      <c r="C96" s="7">
         <f t="shared" si="1"/>
         <v>-7.1236138086586076E-2</v>
       </c>
@@ -4362,9 +4406,9 @@
         <v>38961</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C97" s="5">
+        <v>96</v>
+      </c>
+      <c r="C97" s="7">
         <f t="shared" si="1"/>
         <v>3.8788451160280624E-2</v>
       </c>
@@ -4374,9 +4418,9 @@
         <v>38991</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C98" s="5">
+        <v>97</v>
+      </c>
+      <c r="C98" s="7">
         <f t="shared" si="1"/>
         <v>9.2148840833820356E-2</v>
       </c>
@@ -4386,9 +4430,9 @@
         <v>39022</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C99" s="5">
+        <v>98</v>
+      </c>
+      <c r="C99" s="7">
         <f t="shared" si="1"/>
         <v>-4.9887025805684472E-2</v>
       </c>
@@ -4398,9 +4442,9 @@
         <v>39052</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C100" s="5">
+        <v>99</v>
+      </c>
+      <c r="C100" s="7">
         <f t="shared" si="1"/>
         <v>-3.2292383753676678E-2</v>
       </c>
@@ -4410,9 +4454,9 @@
         <v>39083</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C101" s="5">
+        <v>100</v>
+      </c>
+      <c r="C101" s="7">
         <f t="shared" si="1"/>
         <v>-2.4445450430058857E-2</v>
       </c>
@@ -4422,9 +4466,9 @@
         <v>39114</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C102" s="5">
+        <v>101</v>
+      </c>
+      <c r="C102" s="7">
         <f t="shared" si="1"/>
         <v>1.3987404706662338E-2</v>
       </c>
@@ -4434,9 +4478,9 @@
         <v>39142</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C103" s="5">
+        <v>102</v>
+      </c>
+      <c r="C103" s="7">
         <f t="shared" si="1"/>
         <v>-1.6997907949790756E-2</v>
       </c>
@@ -4446,9 +4490,9 @@
         <v>39173</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C104" s="5">
+        <v>103</v>
+      </c>
+      <c r="C104" s="7">
         <f t="shared" si="1"/>
         <v>-2.4142059058260331E-2</v>
       </c>
@@ -4458,9 +4502,9 @@
         <v>39203</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C105" s="5">
+        <v>104</v>
+      </c>
+      <c r="C105" s="7">
         <f t="shared" si="1"/>
         <v>-1.2744496694608984E-2</v>
       </c>
@@ -4470,9 +4514,9 @@
         <v>39234</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C106" s="5">
+        <v>105</v>
+      </c>
+      <c r="C106" s="7">
         <f t="shared" si="1"/>
         <v>0.14745271296424123</v>
       </c>
@@ -4482,9 +4526,9 @@
         <v>39264</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C107" s="5">
+        <v>106</v>
+      </c>
+      <c r="C107" s="7">
         <f t="shared" si="1"/>
         <v>4.578269762964754E-2</v>
       </c>
@@ -4494,9 +4538,9 @@
         <v>39295</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C108" s="5">
+        <v>107</v>
+      </c>
+      <c r="C108" s="7">
         <f t="shared" si="1"/>
         <v>9.6933785882758972E-2</v>
       </c>
@@ -4506,9 +4550,9 @@
         <v>39326</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C109" s="5">
+        <v>108</v>
+      </c>
+      <c r="C109" s="7">
         <f t="shared" si="1"/>
         <v>0.23258863016572265</v>
       </c>
@@ -4518,9 +4562,9 @@
         <v>39356</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C110" s="5">
+        <v>109</v>
+      </c>
+      <c r="C110" s="7">
         <f t="shared" si="1"/>
         <v>2.3401267923244323E-3</v>
       </c>
@@ -4530,9 +4574,9 @@
         <v>39387</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C111" s="5">
+        <v>110</v>
+      </c>
+      <c r="C111" s="7">
         <f t="shared" si="1"/>
         <v>-6.9615417268019383E-2</v>
       </c>
@@ -4542,9 +4586,9 @@
         <v>39417</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C112" s="5">
+        <v>111</v>
+      </c>
+      <c r="C112" s="7">
         <f t="shared" si="1"/>
         <v>0.15439364905557076</v>
       </c>
@@ -4554,9 +4598,9 @@
         <v>39448</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C113" s="5">
+        <v>112</v>
+      </c>
+      <c r="C113" s="7">
         <f t="shared" si="1"/>
         <v>-7.4697652359497855E-3</v>
       </c>
@@ -4566,9 +4610,9 @@
         <v>39479</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C114" s="5">
+        <v>113</v>
+      </c>
+      <c r="C114" s="7">
         <f t="shared" si="1"/>
         <v>0.14765261020188741</v>
       </c>
@@ -4578,9 +4622,9 @@
         <v>39508</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C115" s="5">
+        <v>114</v>
+      </c>
+      <c r="C115" s="7">
         <f t="shared" si="1"/>
         <v>-1.7174976579577353E-2</v>
       </c>
@@ -4590,9 +4634,9 @@
         <v>39539</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C116" s="5">
+        <v>115</v>
+      </c>
+      <c r="C116" s="7">
         <f t="shared" si="1"/>
         <v>-0.18802513591753156</v>
       </c>
@@ -4602,9 +4646,9 @@
         <v>39569</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C117" s="5">
+        <v>116</v>
+      </c>
+      <c r="C117" s="7">
         <f t="shared" si="1"/>
         <v>-8.1130434782608687E-2</v>
       </c>
@@ -4614,9 +4658,9 @@
         <v>39600</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C118" s="5">
+        <v>117</v>
+      </c>
+      <c r="C118" s="7">
         <f t="shared" si="1"/>
         <v>6.0471278508564402E-2</v>
       </c>
@@ -4626,9 +4670,9 @@
         <v>39630</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C119" s="5">
+        <v>118</v>
+      </c>
+      <c r="C119" s="7">
         <f t="shared" si="1"/>
         <v>-7.1390326610744237E-2</v>
       </c>
@@ -4638,9 +4682,9 @@
         <v>39661</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C120" s="5">
+        <v>119</v>
+      </c>
+      <c r="C120" s="7">
         <f t="shared" si="1"/>
         <v>5.717855083605615E-2</v>
       </c>
@@ -4650,9 +4694,9 @@
         <v>39692</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C121" s="5">
+        <v>120</v>
+      </c>
+      <c r="C121" s="7">
         <f t="shared" si="1"/>
         <v>-6.4948641032633481E-2</v>
       </c>
@@ -4662,9 +4706,9 @@
         <v>39722</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C122" s="5">
+        <v>121</v>
+      </c>
+      <c r="C122" s="7">
         <f t="shared" si="1"/>
         <v>-0.1327468040635785</v>
       </c>
@@ -4674,9 +4718,9 @@
         <v>39753</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C123" s="5">
+        <v>122</v>
+      </c>
+      <c r="C123" s="7">
         <f t="shared" si="1"/>
         <v>-1.2890931509919839E-3</v>
       </c>
@@ -4686,9 +4730,9 @@
         <v>39783</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C124" s="5">
+        <v>123</v>
+      </c>
+      <c r="C124" s="7">
         <f t="shared" si="1"/>
         <v>-7.9353499074022033E-2</v>
       </c>
@@ -4698,9 +4742,9 @@
         <v>39814</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C125" s="5">
+        <v>124</v>
+      </c>
+      <c r="C125" s="7">
         <f t="shared" si="1"/>
         <v>0.10265163060042654</v>
       </c>
@@ -4710,9 +4754,9 @@
         <v>39845</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C126" s="5">
+        <v>125</v>
+      </c>
+      <c r="C126" s="7">
         <f t="shared" si="1"/>
         <v>-2.8359776659848505E-2</v>
       </c>
@@ -4722,9 +4766,9 @@
         <v>39873</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C127" s="5">
+        <v>126</v>
+      </c>
+      <c r="C127" s="7">
         <f t="shared" si="1"/>
         <v>7.908511606736543E-3</v>
       </c>
@@ -4734,9 +4778,9 @@
         <v>39904</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C128" s="5">
+        <v>127</v>
+      </c>
+      <c r="C128" s="7">
         <f t="shared" si="1"/>
         <v>-6.7739204064354807E-4</v>
       </c>
@@ -4746,9 +4790,9 @@
         <v>39934</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C129" s="5">
+        <v>128</v>
+      </c>
+      <c r="C129" s="7">
         <f t="shared" si="1"/>
         <v>6.258826187651817E-2</v>
       </c>
@@ -4758,9 +4802,9 @@
         <v>39965</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C130" s="5">
+        <v>129</v>
+      </c>
+      <c r="C130" s="7">
         <f t="shared" si="1"/>
         <v>-3.8807080963266231E-2</v>
       </c>
@@ -4770,9 +4814,9 @@
         <v>39995</v>
       </c>
       <c r="B131" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C131" s="5">
+        <v>130</v>
+      </c>
+      <c r="C131" s="7">
         <f t="shared" si="1"/>
         <v>-0.11680769868923181</v>
       </c>
@@ -4782,9 +4826,9 @@
         <v>40026</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C132" s="5">
+        <v>131</v>
+      </c>
+      <c r="C132" s="7">
         <f t="shared" si="1"/>
         <v>-7.6648506481307596E-2</v>
       </c>
@@ -4794,9 +4838,9 @@
         <v>40057</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C133" s="5">
+        <v>132</v>
+      </c>
+      <c r="C133" s="7">
         <f t="shared" si="1"/>
         <v>-0.10986775178026442</v>
       </c>
@@ -4806,9 +4850,9 @@
         <v>40087</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C134" s="5">
+        <v>133</v>
+      </c>
+      <c r="C134" s="7">
         <f t="shared" ref="C134:C197" si="2">(B134-B133)/B133</f>
         <v>2.2628571428571422E-2</v>
       </c>
@@ -4818,9 +4862,9 @@
         <v>40118</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C135" s="5">
+        <v>134</v>
+      </c>
+      <c r="C135" s="7">
         <f t="shared" si="2"/>
         <v>5.4313813142601641E-2</v>
       </c>
@@ -4830,9 +4874,9 @@
         <v>40148</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C136" s="5">
+        <v>135</v>
+      </c>
+      <c r="C136" s="7">
         <f t="shared" si="2"/>
         <v>-2.261324288036133E-3</v>
       </c>
@@ -4842,9 +4886,9 @@
         <v>40179</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C137" s="5">
+        <v>136</v>
+      </c>
+      <c r="C137" s="7">
         <f t="shared" si="2"/>
         <v>1.4165309157879619E-4</v>
       </c>
@@ -4854,9 +4898,9 @@
         <v>40210</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C138" s="5">
+        <v>137</v>
+      </c>
+      <c r="C138" s="7">
         <f t="shared" si="2"/>
         <v>6.7275688690601838E-3</v>
       </c>
@@ -4866,9 +4910,9 @@
         <v>40238</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C139" s="5">
+        <v>138</v>
+      </c>
+      <c r="C139" s="7">
         <f t="shared" si="2"/>
         <v>-9.3556555993245926E-3</v>
       </c>
@@ -4878,9 +4922,9 @@
         <v>40269</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C140" s="5">
+        <v>139</v>
+      </c>
+      <c r="C140" s="7">
         <f t="shared" si="2"/>
         <v>2.1373286941702697E-2</v>
       </c>
@@ -4890,9 +4934,9 @@
         <v>40299</v>
       </c>
       <c r="B141" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C141" s="5">
+        <v>140</v>
+      </c>
+      <c r="C141" s="7">
         <f t="shared" si="2"/>
         <v>5.7703003337040053E-3</v>
       </c>
@@ -4902,9 +4946,9 @@
         <v>40330</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C142" s="5">
+        <v>141</v>
+      </c>
+      <c r="C142" s="7">
         <f t="shared" si="2"/>
         <v>-0.10720951130158286</v>
       </c>
@@ -4914,9 +4958,9 @@
         <v>40360</v>
       </c>
       <c r="B143" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C143" s="5">
+        <v>142</v>
+      </c>
+      <c r="C143" s="7">
         <f t="shared" si="2"/>
         <v>0.18759677918860321</v>
       </c>
@@ -4926,9 +4970,9 @@
         <v>40391</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C144" s="5">
+        <v>143</v>
+      </c>
+      <c r="C144" s="7">
         <f t="shared" si="2"/>
         <v>0.24538757415737675</v>
       </c>
@@ -4938,9 +4982,9 @@
         <v>40422</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C145" s="5">
+        <v>144</v>
+      </c>
+      <c r="C145" s="7">
         <f t="shared" si="2"/>
         <v>8.8258388734753626E-2</v>
       </c>
@@ -4950,9 +4994,9 @@
         <v>40452</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C146" s="5">
+        <v>145</v>
+      </c>
+      <c r="C146" s="7">
         <f t="shared" si="2"/>
         <v>-6.4505267208619932E-2</v>
       </c>
@@ -4962,9 +5006,9 @@
         <v>40483</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C147" s="5">
+        <v>146</v>
+      </c>
+      <c r="C147" s="7">
         <f t="shared" si="2"/>
         <v>2.6326614561908705E-2</v>
       </c>
@@ -4974,9 +5018,9 @@
         <v>40513</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C148" s="5">
+        <v>147</v>
+      </c>
+      <c r="C148" s="7">
         <f t="shared" si="2"/>
         <v>0.16177354709418834</v>
       </c>
@@ -4986,9 +5030,9 @@
         <v>40544</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C149" s="5">
+        <v>148</v>
+      </c>
+      <c r="C149" s="7">
         <f t="shared" si="2"/>
         <v>5.429298374229162E-2</v>
       </c>
@@ -4998,9 +5042,9 @@
         <v>40575</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="C150" s="5">
+        <v>149</v>
+      </c>
+      <c r="C150" s="7">
         <f t="shared" si="2"/>
         <v>4.3480039267015803E-2</v>
       </c>
@@ -5010,9 +5054,9 @@
         <v>40603</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C151" s="5">
+        <v>150</v>
+      </c>
+      <c r="C151" s="7">
         <f t="shared" si="2"/>
         <v>-0.11301007408568857</v>
       </c>
@@ -5022,9 +5066,9 @@
         <v>40634</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C152" s="5">
+        <v>151</v>
+      </c>
+      <c r="C152" s="7">
         <f t="shared" si="2"/>
         <v>2.8725472865476401E-2</v>
       </c>
@@ -5034,9 +5078,9 @@
         <v>40664</v>
       </c>
       <c r="B153" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C153" s="5">
+        <v>152</v>
+      </c>
+      <c r="C153" s="7">
         <f t="shared" si="2"/>
         <v>6.1345476415499617E-2</v>
       </c>
@@ -5046,9 +5090,9 @@
         <v>40695</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C154" s="5">
+        <v>153</v>
+      </c>
+      <c r="C154" s="7">
         <f t="shared" si="2"/>
         <v>-8.1640087428155164E-2</v>
       </c>
@@ -5058,9 +5102,9 @@
         <v>40725</v>
       </c>
       <c r="B155" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C155" s="5">
+        <v>154</v>
+      </c>
+      <c r="C155" s="7">
         <f t="shared" si="2"/>
         <v>-6.0205385869804742E-2</v>
       </c>
@@ -5070,9 +5114,9 @@
         <v>40756</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C156" s="5">
+        <v>155</v>
+      </c>
+      <c r="C156" s="7">
         <f t="shared" si="2"/>
         <v>6.9455517516296972E-2</v>
       </c>
@@ -5082,9 +5126,9 @@
         <v>40787</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C157" s="5">
+        <v>156</v>
+      </c>
+      <c r="C157" s="7">
         <f t="shared" si="2"/>
         <v>7.6302403087178091E-3</v>
       </c>
@@ -5094,9 +5138,9 @@
         <v>40817</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="C158" s="5">
+        <v>157</v>
+      </c>
+      <c r="C158" s="7">
         <f t="shared" si="2"/>
         <v>-8.2383149099138339E-2</v>
       </c>
@@ -5106,9 +5150,9 @@
         <v>40848</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C159" s="5">
+        <v>158</v>
+      </c>
+      <c r="C159" s="7">
         <f t="shared" si="2"/>
         <v>-1.8543988617500576E-2</v>
       </c>
@@ -5118,9 +5162,9 @@
         <v>40878</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C160" s="5">
+        <v>159</v>
+      </c>
+      <c r="C160" s="7">
         <f t="shared" si="2"/>
         <v>-1.333719918817044E-2</v>
       </c>
@@ -5130,9 +5174,9 @@
         <v>40909</v>
       </c>
       <c r="B161" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C161" s="5">
+        <v>160</v>
+      </c>
+      <c r="C161" s="7">
         <f t="shared" si="2"/>
         <v>4.2560485845822303E-2</v>
       </c>
@@ -5142,9 +5186,9 @@
         <v>40940</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C162" s="5">
+        <v>161</v>
+      </c>
+      <c r="C162" s="7">
         <f t="shared" si="2"/>
         <v>-1.3012636820594777E-2</v>
       </c>
@@ -5154,9 +5198,9 @@
         <v>40969</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C163" s="5">
+        <v>162</v>
+      </c>
+      <c r="C163" s="7">
         <f t="shared" si="2"/>
         <v>2.356020942408385E-2</v>
       </c>
@@ -5166,9 +5210,9 @@
         <v>41000</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C164" s="5">
+        <v>163</v>
+      </c>
+      <c r="C164" s="7">
         <f t="shared" si="2"/>
         <v>-5.9056033480585989E-2</v>
       </c>
@@ -5178,9 +5222,9 @@
         <v>41030</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C165" s="5">
+        <v>164</v>
+      </c>
+      <c r="C165" s="7">
         <f t="shared" si="2"/>
         <v>2.1003212255992092E-2</v>
       </c>
@@ -5190,9 +5234,9 @@
         <v>41061</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C166" s="5">
+        <v>165</v>
+      </c>
+      <c r="C166" s="7">
         <f t="shared" si="2"/>
         <v>6.7279767666989385E-2</v>
       </c>
@@ -5202,9 +5246,9 @@
         <v>41091</v>
       </c>
       <c r="B167" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C167" s="5">
+        <v>166</v>
+      </c>
+      <c r="C167" s="7">
         <f t="shared" si="2"/>
         <v>0.27727891156462581</v>
       </c>
@@ -5214,9 +5258,9 @@
         <v>41122</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C168" s="5">
+        <v>167</v>
+      </c>
+      <c r="C168" s="7">
         <f t="shared" si="2"/>
         <v>5.6810112199980479E-4</v>
       </c>
@@ -5226,9 +5270,9 @@
         <v>41153</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C169" s="5">
+        <v>168</v>
+      </c>
+      <c r="C169" s="7">
         <f t="shared" si="2"/>
         <v>-2.5443577004968118E-2</v>
       </c>
@@ -5238,9 +5282,9 @@
         <v>41183</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="C170" s="5">
+        <v>169</v>
+      </c>
+      <c r="C170" s="7">
         <f t="shared" si="2"/>
         <v>5.2798310454065054E-3</v>
       </c>
@@ -5250,9 +5294,9 @@
         <v>41214</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C171" s="5">
+        <v>170</v>
+      </c>
+      <c r="C171" s="7">
         <f t="shared" si="2"/>
         <v>1.9994204578383218E-2</v>
       </c>
@@ -5262,9 +5306,9 @@
         <v>41244</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C172" s="5">
+        <v>171</v>
+      </c>
+      <c r="C172" s="7">
         <f t="shared" si="2"/>
         <v>-5.7528409090909248E-2</v>
       </c>
@@ -5274,9 +5318,9 @@
         <v>41275</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C173" s="5">
+        <v>172</v>
+      </c>
+      <c r="C173" s="7">
         <f t="shared" si="2"/>
         <v>-4.8417483044461064E-2</v>
       </c>
@@ -5286,9 +5330,9 @@
         <v>41306</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C174" s="5">
+        <v>173</v>
+      </c>
+      <c r="C174" s="7">
         <f t="shared" si="2"/>
         <v>-5.4603048901207762E-2</v>
       </c>
@@ -5298,9 +5342,9 @@
         <v>41334</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C175" s="5">
+        <v>174</v>
+      </c>
+      <c r="C175" s="7">
         <f t="shared" si="2"/>
         <v>1.3821410621545171E-3</v>
       </c>
@@ -5310,9 +5354,9 @@
         <v>41365</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C176" s="5">
+        <v>175</v>
+      </c>
+      <c r="C176" s="7">
         <f t="shared" si="2"/>
         <v>-8.6160023422142389E-3</v>
       </c>
@@ -5322,9 +5366,9 @@
         <v>41395</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C177" s="5">
+        <v>176</v>
+      </c>
+      <c r="C177" s="7">
         <f t="shared" si="2"/>
         <v>3.6957347171244111E-2</v>
       </c>
@@ -5334,9 +5378,9 @@
         <v>41426</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C178" s="5">
+        <v>177</v>
+      </c>
+      <c r="C178" s="7">
         <f t="shared" si="2"/>
         <v>-3.2751535863948834E-2</v>
       </c>
@@ -5346,9 +5390,9 @@
         <v>41456</v>
       </c>
       <c r="B179" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C179" s="5">
+        <v>178</v>
+      </c>
+      <c r="C179" s="7">
         <f t="shared" si="2"/>
         <v>-2.0442500210313845E-2</v>
       </c>
@@ -5358,9 +5402,9 @@
         <v>41487</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C180" s="5">
+        <v>179</v>
+      </c>
+      <c r="C180" s="7">
         <f t="shared" si="2"/>
         <v>-1.4385091034008908E-2</v>
       </c>
@@ -5370,9 +5414,9 @@
         <v>41518</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C181" s="5">
+        <v>180</v>
+      </c>
+      <c r="C181" s="7">
         <f t="shared" si="2"/>
         <v>3.3111140155970501E-3</v>
       </c>
@@ -5382,9 +5426,9 @@
         <v>41548</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C182" s="5">
+        <v>181</v>
+      </c>
+      <c r="C182" s="7">
         <f t="shared" si="2"/>
         <v>3.5086195666333808E-2</v>
       </c>
@@ -5394,9 +5438,9 @@
         <v>41579</v>
       </c>
       <c r="B183" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C183" s="5">
+        <v>182</v>
+      </c>
+      <c r="C183" s="7">
         <f t="shared" si="2"/>
         <v>-4.5433569660611704E-2</v>
       </c>
@@ -5406,9 +5450,9 @@
         <v>41609</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C184" s="5">
+        <v>183</v>
+      </c>
+      <c r="C184" s="7">
         <f t="shared" si="2"/>
         <v>-6.4604025665816953E-2</v>
       </c>
@@ -5418,9 +5462,9 @@
         <v>41640</v>
       </c>
       <c r="B185" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C185" s="5">
+        <v>184</v>
+      </c>
+      <c r="C185" s="7">
         <f t="shared" si="2"/>
         <v>-0.21231911294869385</v>
       </c>
@@ -5430,9 +5474,9 @@
         <v>41671</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C186" s="5">
+        <v>185</v>
+      </c>
+      <c r="C186" s="7">
         <f t="shared" si="2"/>
         <v>6.0363853265732202E-2</v>
       </c>
@@ -5442,9 +5486,9 @@
         <v>41699</v>
       </c>
       <c r="B187" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C187" s="5">
+        <v>186</v>
+      </c>
+      <c r="C187" s="7">
         <f t="shared" si="2"/>
         <v>0.12150531585756873</v>
       </c>
@@ -5454,9 +5498,9 @@
         <v>41730</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="C188" s="5">
+        <v>187</v>
+      </c>
+      <c r="C188" s="7">
         <f t="shared" si="2"/>
         <v>-6.9218036815970078E-3</v>
       </c>
@@ -5466,9 +5510,9 @@
         <v>41760</v>
       </c>
       <c r="B189" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C189" s="5">
+        <v>188</v>
+      </c>
+      <c r="C189" s="7">
         <f t="shared" si="2"/>
         <v>5.84372948128693E-2</v>
       </c>
@@ -5478,9 +5522,9 @@
         <v>41791</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="C190" s="5">
+        <v>189</v>
+      </c>
+      <c r="C190" s="7">
         <f t="shared" si="2"/>
         <v>-8.1599541897308614E-2</v>
       </c>
@@ -5490,9 +5534,9 @@
         <v>41821</v>
       </c>
       <c r="B191" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C191" s="5">
+        <v>190</v>
+      </c>
+      <c r="C191" s="7">
         <f t="shared" si="2"/>
         <v>-8.4744882053413711E-2</v>
       </c>
@@ -5502,9 +5546,9 @@
         <v>41852</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C192" s="5">
+        <v>191</v>
+      </c>
+      <c r="C192" s="7">
         <f t="shared" si="2"/>
         <v>-2.3275617371558296E-2</v>
       </c>
@@ -5514,9 +5558,9 @@
         <v>41883</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C193" s="5">
+        <v>192</v>
+      </c>
+      <c r="C193" s="7">
         <f t="shared" si="2"/>
         <v>-4.7776809067131637E-2</v>
       </c>
@@ -5526,9 +5570,9 @@
         <v>41913</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C194" s="5">
+        <v>193</v>
+      </c>
+      <c r="C194" s="7">
         <f t="shared" si="2"/>
         <v>2.4903863761215797E-2</v>
       </c>
@@ -5538,9 +5582,9 @@
         <v>41944</v>
       </c>
       <c r="B195" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C195" s="5">
+        <v>194</v>
+      </c>
+      <c r="C195" s="7">
         <f t="shared" si="2"/>
         <v>3.1266750044666787E-2</v>
       </c>
@@ -5550,9 +5594,9 @@
         <v>41974</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="C196" s="5">
+        <v>195</v>
+      </c>
+      <c r="C196" s="7">
         <f t="shared" si="2"/>
         <v>9.1129591129591139E-2</v>
       </c>
@@ -5562,9 +5606,9 @@
         <v>42005</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C197" s="5">
+        <v>196</v>
+      </c>
+      <c r="C197" s="7">
         <f t="shared" si="2"/>
         <v>-3.8636604212977724E-2</v>
       </c>
@@ -5574,9 +5618,9 @@
         <v>42036</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C198" s="5">
+        <v>197</v>
+      </c>
+      <c r="C198" s="7">
         <f t="shared" ref="C198:C211" si="3">(B198-B197)/B197</f>
         <v>-2.1250825809293026E-2</v>
       </c>
@@ -5586,9 +5630,9 @@
         <v>42064</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C199" s="5">
+        <v>198</v>
+      </c>
+      <c r="C199" s="7">
         <f t="shared" si="3"/>
         <v>5.2311846101923791E-2</v>
       </c>
@@ -5598,9 +5642,9 @@
         <v>42095</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C200" s="5">
+        <v>199</v>
+      </c>
+      <c r="C200" s="7">
         <f t="shared" si="3"/>
         <v>-2.8383579217447091E-2</v>
       </c>
@@ -5610,9 +5654,9 @@
         <v>42125</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C201" s="5">
+        <v>200</v>
+      </c>
+      <c r="C201" s="7">
         <f t="shared" si="3"/>
         <v>-4.753259613797664E-2</v>
       </c>
@@ -5622,9 +5666,9 @@
         <v>42156</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C202" s="5">
+        <v>201</v>
+      </c>
+      <c r="C202" s="7">
         <f t="shared" si="3"/>
         <v>2.9342112863166479E-2</v>
       </c>
@@ -5634,9 +5678,9 @@
         <v>42186</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C203" s="5">
+        <v>202</v>
+      </c>
+      <c r="C203" s="7">
         <f t="shared" si="3"/>
         <v>1.7058526457550037E-2</v>
       </c>
@@ -5646,9 +5690,9 @@
         <v>42217</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C204" s="5">
+        <v>203</v>
+      </c>
+      <c r="C204" s="7">
         <f t="shared" si="3"/>
         <v>-0.14057931034482754</v>
       </c>
@@ -5658,9 +5702,9 @@
         <v>42248</v>
       </c>
       <c r="B205" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C205" s="5">
+        <v>204</v>
+      </c>
+      <c r="C205" s="7">
         <f t="shared" si="3"/>
         <v>-6.2977466777941846E-2</v>
       </c>
@@ -5670,9 +5714,9 @@
         <v>42278</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C206" s="5">
+        <v>205</v>
+      </c>
+      <c r="C206" s="7">
         <f t="shared" si="3"/>
         <v>9.3176212661001991E-3</v>
       </c>
@@ -5682,9 +5726,9 @@
         <v>42309</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C207" s="5">
+        <v>206</v>
+      </c>
+      <c r="C207" s="7">
         <f t="shared" si="3"/>
         <v>-3.9370078740156404E-3</v>
       </c>
@@ -5694,9 +5738,9 @@
         <v>42339</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C208" s="5">
+        <v>207</v>
+      </c>
+      <c r="C208" s="7">
         <f t="shared" si="3"/>
         <v>2.6305029303529952E-2</v>
       </c>
@@ -5706,9 +5750,9 @@
         <v>42370</v>
       </c>
       <c r="B209" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C209" s="5">
+        <v>208</v>
+      </c>
+      <c r="C209" s="7">
         <f t="shared" si="3"/>
         <v>6.3745019920319257E-3</v>
       </c>
@@ -5718,9 +5762,9 @@
         <v>42401</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C210" s="5">
+        <v>209</v>
+      </c>
+      <c r="C210" s="7">
         <f t="shared" si="3"/>
         <v>-5.2256532066508418E-2</v>
       </c>
@@ -5730,9 +5774,9 @@
         <v>42430</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C211" s="5">
+        <v>210</v>
+      </c>
+      <c r="C211" s="7">
         <f t="shared" si="3"/>
         <v>2.9030910609858091E-2</v>
       </c>

</xml_diff>